<commit_message>
mini instance works kindaaa?
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -465,10 +465,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2142857142857143</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -478,10 +478,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3" t="n">
         <v>3</v>
@@ -494,13 +494,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>